<commit_message>
can edit one by one
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SW2137\source\repos\ExcelDataEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD439E1F-920C-4AF5-BABB-3D1880A4EFCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1B31E1-9607-4FA6-B723-6C3EC1133CBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19535" windowHeight="9007" xr2:uid="{907BBAF0-D6AB-4F10-9431-D3C4BA3C78FA}"/>
   </bookViews>
@@ -25,9 +25,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>1m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023-03-15 오후 1:47:14</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -392,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F491EB0A-EC98-41CC-9A91-A5E66BA10D5E}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -609,6 +613,11 @@
         <v>100</v>
       </c>
     </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
copy and paste success
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SW2137\source\repos\ExcelDataEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1B31E1-9607-4FA6-B723-6C3EC1133CBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D987323-416A-4578-8730-D8AAE7BD2F53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19535" windowHeight="9007" xr2:uid="{907BBAF0-D6AB-4F10-9431-D3C4BA3C78FA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2023-03-15 오후 1:47:14</t>
+    <t>2023-03-16 오전 8:27:04</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -396,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F491EB0A-EC98-41CC-9A91-A5E66BA10D5E}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -618,6 +618,103 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>45</v>
+      </c>
+      <c r="D11">
+        <v>60</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0.3</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>0.7</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>0.2</v>
+      </c>
+      <c r="C13">
+        <v>0.3</v>
+      </c>
+      <c r="D13">
+        <v>0.4</v>
+      </c>
+      <c r="E13">
+        <v>0.6</v>
+      </c>
+      <c r="F13">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>0.12</v>
+      </c>
+      <c r="C14">
+        <v>0.18</v>
+      </c>
+      <c r="D14">
+        <v>0.26</v>
+      </c>
+      <c r="E14">
+        <v>0.4</v>
+      </c>
+      <c r="F14">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>80</v>
+      </c>
+      <c r="B15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C15">
+        <v>0.13</v>
+      </c>
+      <c r="D15">
+        <v>0.18</v>
+      </c>
+      <c r="E15">
+        <v>0.31</v>
+      </c>
+      <c r="F15">
+        <v>0.65</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>